<commit_message>
updated sample subscriber data
</commit_message>
<xml_diff>
--- a/sample_data/sample_subscriber_data.xlsx
+++ b/sample_data/sample_subscriber_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/od685f/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/od685f/Documents/Repositories/python-tutorials/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFAEAEE4-09B1-6E43-AB24-FDA1333D4E30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C771955-9B2D-C64B-BD73-B4226DED7312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14500" yWindow="460" windowWidth="19100" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>acct_num</t>
   </si>
@@ -121,9 +121,6 @@
     <t>4524 Nickel Road</t>
   </si>
   <si>
-    <t>New YorkLos Angeles</t>
-  </si>
-  <si>
     <t>CA</t>
   </si>
   <si>
@@ -212,6 +209,12 @@
   </si>
   <si>
     <t>OH</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>product_qty</t>
   </si>
 </sst>
 </file>
@@ -600,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +623,7 @@
     <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,8 +651,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -673,8 +679,11 @@
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -698,8 +707,11 @@
       <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -723,8 +735,11 @@
       <c r="I4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -736,10 +751,10 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G5" s="1">
         <v>90017</v>
@@ -748,23 +763,26 @@
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G6" s="1">
         <v>37160</v>
@@ -773,23 +791,26 @@
       <c r="I6" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="G7" s="1">
         <v>33417</v>
@@ -798,23 +819,26 @@
       <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="G8" s="1">
         <v>93308</v>
@@ -823,23 +847,26 @@
       <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="1">
         <v>95926</v>
@@ -848,20 +875,23 @@
       <c r="I9" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>13</v>
@@ -873,23 +903,26 @@
       <c r="I10" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="1">
         <v>37601</v>
@@ -898,23 +931,26 @@
       <c r="I11" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="G12" s="1">
         <v>8901</v>
@@ -923,23 +959,26 @@
       <c r="I12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="G13" s="1">
         <v>44115</v>
@@ -947,6 +986,9 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="J13">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>